<commit_message>
bug fixes and requirements
</commit_message>
<xml_diff>
--- a/requirements/CQs.xlsx
+++ b/requirements/CQs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>CQ id</t>
   </si>
@@ -88,6 +88,39 @@
   </si>
   <si>
     <t>What is the high-level workflow associated to an ensemble?</t>
+  </si>
+  <si>
+    <t>What is the specification of an ensemble?</t>
+  </si>
+  <si>
+    <t>What is the ensemble specification of an ensemble?</t>
+  </si>
+  <si>
+    <t>What is the region associated to a modeling question?</t>
+  </si>
+  <si>
+    <t>What are the ensemble specifications of a modeling question?</t>
+  </si>
+  <si>
+    <t>What are the ensembles of a modeling question?</t>
+  </si>
+  <si>
+    <t>Which data was selected to run the ensembles in a modeling question?</t>
+  </si>
+  <si>
+    <t>Which interventions are associated to a modeling question?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which values in particular were changed in as part of an intervention in the realizations of an ensemble? </t>
+  </si>
+  <si>
+    <t>What is the theme of an ensemble?</t>
+  </si>
+  <si>
+    <t>What are the templates associated to an ensemble?</t>
+  </si>
+  <si>
+    <t>What are the workflow templates associated to a modeling question?</t>
   </si>
 </sst>
 </file>
@@ -407,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,55 +538,88 @@
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>